<commit_message>
New_LL_All Modules without biometrics and slot result
</commit_message>
<xml_diff>
--- a/RunManager.xlsx
+++ b/RunManager.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\Framework_fileupload\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="13275" windowHeight="10230"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="9" r:id="rId1"/>
-    <sheet name="IterationOptions" sheetId="10" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId2"/>
+    <sheet name="IterationOptions" sheetId="10" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$F$179</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$F$175</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Execute</t>
   </si>
@@ -93,12 +99,51 @@
   </si>
   <si>
     <t>File_Upoad</t>
+  </si>
+  <si>
+    <t>ApplyLLApplication</t>
+  </si>
+  <si>
+    <t>New LLSubmission</t>
+  </si>
+  <si>
+    <t>LL_SlotBooking</t>
+  </si>
+  <si>
+    <t>Slot Bokking for LL</t>
+  </si>
+  <si>
+    <t>New_LLSubmission_slotbooking_fee_payment</t>
+  </si>
+  <si>
+    <t>Fee_Payment</t>
+  </si>
+  <si>
+    <t>Pay fee for New LL</t>
+  </si>
+  <si>
+    <t>Upload_photo_signature</t>
+  </si>
+  <si>
+    <t>Upload_photo_and_Signature</t>
+  </si>
+  <si>
+    <t>Upload_photo_signature process</t>
+  </si>
+  <si>
+    <t>Scrutinie_action</t>
+  </si>
+  <si>
+    <t>Scrutinie of new LL</t>
+  </si>
+  <si>
+    <t>New_LL_Scrutinie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -160,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -174,12 +219,23 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -226,7 +282,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,9 +314,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,6 +349,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,12 +525,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Scenario1"/>
-  <dimension ref="A1:F179"/>
+  <dimension ref="A1:F175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -508,10 +566,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -523,15 +581,15 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
+      <c r="A3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -543,15 +601,15 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
+      <c r="A4" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -563,15 +621,15 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
+      <c r="A5" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -583,31 +641,48 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="D7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="D8" s="2"/>
@@ -1113,42 +1188,137 @@
     <row r="175" spans="4:4">
       <c r="D175" s="2"/>
     </row>
-    <row r="176" spans="4:4">
-      <c r="D176" s="2"/>
-    </row>
-    <row r="177" spans="4:4">
-      <c r="D177" s="2"/>
-    </row>
-    <row r="178" spans="4:4">
-      <c r="D178" s="2"/>
-    </row>
-    <row r="179" spans="4:4">
-      <c r="D179" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F179"/>
+  <autoFilter ref="A1:F175"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
-      <formula1>"Module1,Module2,Module3"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D179">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D175">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C179">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C175">
       <formula1>"firefox,internetexplorer,chrome"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E20">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E16">
       <formula1>"All Iterations,1-2,1-3,1-4,1,2,3,4"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" sqref="E1:E4">
+      <formula1>"All Iterations,1-2,1-3,1-4,1,2,3,4"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C4">
+      <formula1>"firefox,internetexplorer,chrome"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D4">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F4">
+      <formula1>"Module1,Module2,Module3"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="IterationOptions"/>
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Up To 14-11-2017 Sarathi project By using This FW
</commit_message>
<xml_diff>
--- a/RunManager.xlsx
+++ b/RunManager.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>Execute</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Upload_File</t>
   </si>
   <si>
-    <t>file upload</t>
-  </si>
-  <si>
     <t>File_Upoad</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>Upload_photo_and_Signature</t>
   </si>
   <si>
-    <t>Upload_photo_signature process</t>
-  </si>
-  <si>
     <t>Scrutinie_action</t>
   </si>
   <si>
@@ -138,6 +132,63 @@
   </si>
   <si>
     <t>New_LL_Scrutinie</t>
+  </si>
+  <si>
+    <t>file upload_LL</t>
+  </si>
+  <si>
+    <t>Upload_photo_signature process_LL</t>
+  </si>
+  <si>
+    <t>DL_Submission</t>
+  </si>
+  <si>
+    <t>Apply DL_form_Submission</t>
+  </si>
+  <si>
+    <t>Apply_DL_Submission</t>
+  </si>
+  <si>
+    <t>DL_Services</t>
+  </si>
+  <si>
+    <t>Edit on DL_Services Back Log</t>
+  </si>
+  <si>
+    <t>DL_Back_Logs</t>
+  </si>
+  <si>
+    <t>Dl_Page Submission</t>
+  </si>
+  <si>
+    <t>DL_Page_Submission</t>
+  </si>
+  <si>
+    <t>DL_Page_Data_Filling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dl_Services_Changes </t>
+  </si>
+  <si>
+    <t>Services_On_Dl</t>
+  </si>
+  <si>
+    <t>DL_Backlog_services</t>
+  </si>
+  <si>
+    <t>DL_servces_withoutlogin</t>
+  </si>
+  <si>
+    <t>DL_Backlog</t>
+  </si>
+  <si>
+    <t>LL_BackLog</t>
+  </si>
+  <si>
+    <t>LL_Backlog</t>
+  </si>
+  <si>
+    <t>LL_Services_Backlog</t>
   </si>
 </sst>
 </file>
@@ -530,7 +581,7 @@
   <dimension ref="A1:F175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -569,7 +620,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -581,15 +632,15 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -601,15 +652,15 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -621,15 +672,15 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -641,15 +692,15 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -661,46 +712,148 @@
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="D8" s="2"/>
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="D9" s="2"/>
+      <c r="A9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="D10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="D11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="D12" s="2"/>
+      <c r="A12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="D13" s="2"/>
+      <c r="A13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="D14" s="2"/>
@@ -1213,7 +1366,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>